<commit_message>
[improvements] - improve performance of preparing and validating large plan files (multiple subplans and many steps)
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_numberCommand.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_numberCommand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\src\test\resources\unittesting\artifact\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B91661-012A-4B13-952B-F0DAA3B95159}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D563E7-40DA-489C-9060-25DE134168F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="663">
   <si>
     <t>target</t>
   </si>
@@ -2030,6 +2030,27 @@
   </si>
   <si>
     <t>${num3}</t>
+  </si>
+  <si>
+    <t>more rounding tests</t>
+  </si>
+  <si>
+    <t>[NUMBER(1.49) =&gt; roundTo(0)]</t>
+  </si>
+  <si>
+    <t>[NUMBER(1.49) =&gt; roundTo(0.0)]</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>consider 2nd dec. places</t>
+  </si>
+  <si>
+    <t>ignore 2nd dec. places</t>
   </si>
 </sst>
 </file>
@@ -4749,14 +4770,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O1035"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.25" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.5" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="33.625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
@@ -6823,22 +6844,135 @@
         <v>655</v>
       </c>
     </row>
-    <row r="113" ht="18.75" customHeight="1"/>
-    <row r="114" ht="18.75" customHeight="1"/>
-    <row r="115" ht="18.75" customHeight="1"/>
-    <row r="116" ht="18.75" customHeight="1"/>
-    <row r="117" ht="18.75" customHeight="1"/>
-    <row r="118" ht="18.75" customHeight="1"/>
-    <row r="119" ht="18.75" customHeight="1"/>
-    <row r="120" ht="18.75" customHeight="1"/>
-    <row r="121" ht="18.75" customHeight="1"/>
-    <row r="122" ht="18.75" customHeight="1"/>
-    <row r="123" ht="18.75" customHeight="1"/>
-    <row r="124" ht="18.75" customHeight="1"/>
-    <row r="125" ht="18.75" customHeight="1"/>
-    <row r="126" ht="18.75" customHeight="1"/>
-    <row r="127" ht="18.75" customHeight="1"/>
-    <row r="128" ht="18.75" customHeight="1"/>
+    <row r="113" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A113" s="13" t="s">
+        <v>656</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="F113" s="19" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="18.75" customHeight="1">
+      <c r="C114" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="18.75" customHeight="1">
+      <c r="C115" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="F115" s="19" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="18.75" customHeight="1">
+      <c r="C116" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="18.75" customHeight="1">
+      <c r="C117" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="F117" s="19" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="18.75" customHeight="1">
+      <c r="C118" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="18.75" customHeight="1">
+      <c r="B119" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="F119" s="19" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="18.75" customHeight="1">
+      <c r="C120" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="18.75" customHeight="1"/>
+    <row r="122" spans="1:6" ht="18.75" customHeight="1"/>
+    <row r="123" spans="1:6" ht="18.75" customHeight="1"/>
+    <row r="124" spans="1:6" ht="18.75" customHeight="1"/>
+    <row r="125" spans="1:6" ht="18.75" customHeight="1"/>
+    <row r="126" spans="1:6" ht="18.75" customHeight="1"/>
+    <row r="127" spans="1:6" ht="18.75" customHeight="1"/>
+    <row r="128" spans="1:6" ht="18.75" customHeight="1"/>
     <row r="129" ht="18.75" customHeight="1"/>
     <row r="130" ht="18.75" customHeight="1"/>
     <row r="131" ht="18.75" customHeight="1"/>

</xml_diff>